<commit_message>
Auth routes for UserTypes
</commit_message>
<xml_diff>
--- a/docs/DisenoAPIBedushop.xlsx
+++ b/docs/DisenoAPIBedushop.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="97">
   <si>
     <t xml:space="preserve">Path version 1</t>
   </si>
@@ -257,6 +257,24 @@
   </si>
   <si>
     <t xml:space="preserve">Get all products in orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get all userTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Usertype by Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new userType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATE userTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE UserType</t>
   </si>
   <si>
     <t xml:space="preserve">ID endpoint</t>
@@ -590,15 +608,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.87"/>
   </cols>
@@ -1630,11 +1649,19 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -1644,11 +1671,19 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -1658,11 +1693,19 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -1671,15 +1714,20 @@
       <c r="L43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -1688,16 +1736,20 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -1706,16 +1758,20 @@
       <c r="L45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="16" t="n">
-        <v>44713</v>
-      </c>
+      <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -1724,64 +1780,117 @@
       <c r="L46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="A47" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="B47" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>37</v>
+      <c r="A48" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>31</v>
+      <c r="A49" s="16" t="n">
+        <v>44713</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="16" t="n">
-        <v>44713</v>
+      <c r="A50" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="n">
+      <c r="A52" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="16" t="n">
+        <v>44713</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
+      <c r="B55" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
added initial access and updated routes
</commit_message>
<xml_diff>
--- a/docs/DisenoAPIBedushop.xlsx
+++ b/docs/DisenoAPIBedushop.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="97">
   <si>
     <t xml:space="preserve">Path version 1</t>
   </si>
@@ -257,6 +257,24 @@
   </si>
   <si>
     <t xml:space="preserve">Get all products in orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get all userTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get Usertype by Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create new userType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDATE userTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE UserType</t>
   </si>
   <si>
     <t xml:space="preserve">ID endpoint</t>
@@ -590,15 +608,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J44" activeCellId="0" sqref="J44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.87"/>
   </cols>
@@ -1630,11 +1649,19 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -1644,11 +1671,19 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -1658,11 +1693,19 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -1671,15 +1714,20 @@
       <c r="L43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B44" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C44" s="15"/>
+      <c r="C44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -1688,16 +1736,20 @@
       <c r="L44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -1706,16 +1758,20 @@
       <c r="L45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="16" t="n">
-        <v>44713</v>
-      </c>
+      <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -1724,64 +1780,117 @@
       <c r="L46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="A47" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
+      <c r="B47" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="n">
-        <v>37</v>
+      <c r="A48" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="n">
-        <v>31</v>
+      <c r="A49" s="16" t="n">
+        <v>44713</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="16" t="n">
-        <v>44713</v>
+      <c r="A50" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="n">
+      <c r="A52" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="16" t="n">
+        <v>44713</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B52" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="9"/>
+      <c r="B55" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>